<commit_message>
version alpha done !
</commit_message>
<xml_diff>
--- a/public/Rapport-2017-11-11.xlsx
+++ b/public/Rapport-2017-11-11.xlsx
@@ -621,211 +621,153 @@
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="3">
-        <v>25</v>
-      </c>
+      <c r="B2" s="3"/>
       <c r="C2" s="3">
         <v>133</v>
       </c>
-      <c r="D2" s="3">
-        <v>18.8</v>
-      </c>
+      <c r="D2" s="3"/>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="3">
-        <v>7</v>
-      </c>
+      <c r="B3" s="3"/>
       <c r="C3" s="3">
         <v>84</v>
       </c>
-      <c r="D3" s="3">
-        <v>8.33</v>
-      </c>
+      <c r="D3" s="3"/>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="3">
-        <v>18</v>
-      </c>
+      <c r="B4" s="3"/>
       <c r="C4" s="3">
         <v>107</v>
       </c>
-      <c r="D4" s="3">
-        <v>16.82</v>
-      </c>
+      <c r="D4" s="3"/>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="3">
-        <v>10</v>
-      </c>
+      <c r="B5" s="3"/>
       <c r="C5" s="3">
         <v>25</v>
       </c>
-      <c r="D5" s="3">
-        <v>40</v>
-      </c>
+      <c r="D5" s="3"/>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="3">
-        <v>11</v>
-      </c>
+      <c r="B6" s="3"/>
       <c r="C6" s="3">
         <v>98</v>
       </c>
-      <c r="D6" s="3">
-        <v>11.22</v>
-      </c>
+      <c r="D6" s="3"/>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="3">
-        <v>5</v>
-      </c>
+      <c r="B7" s="3"/>
       <c r="C7" s="3">
         <v>27</v>
       </c>
-      <c r="D7" s="3">
-        <v>18.52</v>
-      </c>
+      <c r="D7" s="3"/>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="3">
-        <v>15</v>
-      </c>
+      <c r="B8" s="3"/>
       <c r="C8" s="3">
         <v>39</v>
       </c>
-      <c r="D8" s="3">
-        <v>38.46</v>
-      </c>
+      <c r="D8" s="3"/>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="3">
-        <v>11</v>
-      </c>
+      <c r="B9" s="3"/>
       <c r="C9" s="3">
         <v>87</v>
       </c>
-      <c r="D9" s="3">
-        <v>12.64</v>
-      </c>
+      <c r="D9" s="3"/>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="3">
-        <v>11</v>
-      </c>
+      <c r="B10" s="3"/>
       <c r="C10" s="3">
         <v>46</v>
       </c>
-      <c r="D10" s="3">
-        <v>23.91</v>
-      </c>
+      <c r="D10" s="3"/>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="3">
-        <v>10</v>
-      </c>
+      <c r="B11" s="3"/>
       <c r="C11" s="3">
         <v>78</v>
       </c>
-      <c r="D11" s="3">
-        <v>12.82</v>
-      </c>
+      <c r="D11" s="3"/>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="3">
-        <v>11</v>
-      </c>
+      <c r="B12" s="3"/>
       <c r="C12" s="3">
         <v>50</v>
       </c>
-      <c r="D12" s="3">
-        <v>22</v>
-      </c>
+      <c r="D12" s="3"/>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="3">
-        <v>13</v>
-      </c>
+      <c r="B13" s="3"/>
       <c r="C13" s="3">
         <v>70</v>
       </c>
-      <c r="D13" s="3">
-        <v>18.57</v>
-      </c>
+      <c r="D13" s="3"/>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="3">
-        <v>3</v>
-      </c>
+      <c r="B14" s="3"/>
       <c r="C14" s="3">
         <v>4</v>
       </c>
-      <c r="D14" s="3">
-        <v>75</v>
-      </c>
+      <c r="D14" s="3"/>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="3">
-        <v>5</v>
-      </c>
+      <c r="B15" s="3"/>
       <c r="C15" s="3">
         <v>33</v>
       </c>
-      <c r="D15" s="3">
-        <v>15.15</v>
-      </c>
+      <c r="D15" s="3"/>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B16" s="3">
-        <v>77</v>
+        <v>0</v>
       </c>
       <c r="C16" s="3">
-        <v>413</v>
-      </c>
-      <c r="D16" s="3">
-        <v>18.64</v>
-      </c>
+        <v>310</v>
+      </c>
+      <c r="D16" s="3"/>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="2"/>
@@ -888,7 +830,7 @@
       </c>
       <c r="B2" s="6">
         <f>SUM(C4:C2000)</f>
-        <v>155</v>
+        <v>0</v>
       </c>
       <c r="C2" s="6">
         <f>SUM(D4:D2000)</f>
@@ -896,7 +838,7 @@
       </c>
       <c r="D2" s="6">
         <f>ROUND(((B2/C2)*100),2)</f>
-        <v>17.59</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:5" customHeight="1" ht="45">
@@ -905,7 +847,7 @@
       </c>
       <c r="B3" s="5">
         <f>SUBTOTAL(109,C4:C2000)</f>
-        <v>155</v>
+        <v>0</v>
       </c>
       <c r="C3" s="5">
         <f>SUBTOTAL(109,D4:D2000)</f>
@@ -913,7 +855,7 @@
       </c>
       <c r="D3" s="5">
         <f>ROUND(((B3/C3)*100),2)</f>
-        <v>17.59</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:5" customHeight="1" ht="30">
@@ -1039,9 +981,7 @@
       <c r="B15" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C15" s="3">
-        <v>1</v>
-      </c>
+      <c r="C15" s="3"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
     </row>
@@ -1078,15 +1018,11 @@
       <c r="B18" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C18" s="3">
-        <v>2</v>
-      </c>
+      <c r="C18" s="3"/>
       <c r="D18" s="3">
         <v>13</v>
       </c>
-      <c r="E18" s="3">
-        <v>15</v>
-      </c>
+      <c r="E18" s="3"/>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="3" t="s">
@@ -1108,15 +1044,11 @@
       <c r="B20" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C20" s="3">
-        <v>3</v>
-      </c>
+      <c r="C20" s="3"/>
       <c r="D20" s="3">
         <v>8</v>
       </c>
-      <c r="E20" s="3">
-        <v>38</v>
-      </c>
+      <c r="E20" s="3"/>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="3" t="s">
@@ -1125,15 +1057,11 @@
       <c r="B21" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C21" s="3">
-        <v>7</v>
-      </c>
+      <c r="C21" s="3"/>
       <c r="D21" s="3">
         <v>23</v>
       </c>
-      <c r="E21" s="3">
-        <v>30</v>
-      </c>
+      <c r="E21" s="3"/>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="3" t="s">
@@ -1142,15 +1070,11 @@
       <c r="B22" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C22" s="3">
-        <v>1</v>
-      </c>
+      <c r="C22" s="3"/>
       <c r="D22" s="3">
         <v>38</v>
       </c>
-      <c r="E22" s="3">
-        <v>3</v>
-      </c>
+      <c r="E22" s="3"/>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="3" t="s">
@@ -1159,15 +1083,11 @@
       <c r="B23" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C23" s="3">
-        <v>4</v>
-      </c>
+      <c r="C23" s="3"/>
       <c r="D23" s="3">
         <v>22</v>
       </c>
-      <c r="E23" s="3">
-        <v>18</v>
-      </c>
+      <c r="E23" s="3"/>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="3" t="s">
@@ -1176,15 +1096,11 @@
       <c r="B24" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C24" s="3">
-        <v>6</v>
-      </c>
+      <c r="C24" s="3"/>
       <c r="D24" s="3">
         <v>10</v>
       </c>
-      <c r="E24" s="3">
-        <v>60</v>
-      </c>
+      <c r="E24" s="3"/>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="3" t="s">
@@ -1193,15 +1109,11 @@
       <c r="B25" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C25" s="3">
-        <v>1</v>
-      </c>
+      <c r="C25" s="3"/>
       <c r="D25" s="3">
         <v>6</v>
       </c>
-      <c r="E25" s="3">
-        <v>17</v>
-      </c>
+      <c r="E25" s="3"/>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="3" t="s">
@@ -1353,15 +1265,11 @@
       <c r="B39" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C39" s="3">
-        <v>1</v>
-      </c>
+      <c r="C39" s="3"/>
       <c r="D39" s="3">
         <v>4</v>
       </c>
-      <c r="E39" s="3">
-        <v>25</v>
-      </c>
+      <c r="E39" s="3"/>
     </row>
     <row r="40" spans="1:5">
       <c r="A40" s="3" t="s">
@@ -1396,15 +1304,11 @@
       <c r="B42" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C42" s="3">
-        <v>1</v>
-      </c>
+      <c r="C42" s="3"/>
       <c r="D42" s="3">
         <v>6</v>
       </c>
-      <c r="E42" s="3">
-        <v>17</v>
-      </c>
+      <c r="E42" s="3"/>
     </row>
     <row r="43" spans="1:5">
       <c r="A43" s="3" t="s">
@@ -1426,15 +1330,11 @@
       <c r="B44" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C44" s="3">
-        <v>1</v>
-      </c>
+      <c r="C44" s="3"/>
       <c r="D44" s="3">
         <v>7</v>
       </c>
-      <c r="E44" s="3">
-        <v>14</v>
-      </c>
+      <c r="E44" s="3"/>
     </row>
     <row r="45" spans="1:5">
       <c r="A45" s="3" t="s">
@@ -1456,15 +1356,11 @@
       <c r="B46" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C46" s="3">
-        <v>2</v>
-      </c>
+      <c r="C46" s="3"/>
       <c r="D46" s="3">
         <v>9</v>
       </c>
-      <c r="E46" s="3">
-        <v>22</v>
-      </c>
+      <c r="E46" s="3"/>
     </row>
     <row r="47" spans="1:5">
       <c r="A47" s="3" t="s">
@@ -1486,15 +1382,11 @@
       <c r="B48" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C48" s="3">
-        <v>2</v>
-      </c>
+      <c r="C48" s="3"/>
       <c r="D48" s="3">
         <v>6</v>
       </c>
-      <c r="E48" s="3">
-        <v>33</v>
-      </c>
+      <c r="E48" s="3"/>
     </row>
     <row r="49" spans="1:5">
       <c r="A49" s="3" t="s">
@@ -1670,15 +1562,11 @@
       <c r="B64" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C64" s="3">
-        <v>1</v>
-      </c>
+      <c r="C64" s="3"/>
       <c r="D64" s="3">
         <v>1</v>
       </c>
-      <c r="E64" s="3">
-        <v>100</v>
-      </c>
+      <c r="E64" s="3"/>
     </row>
     <row r="65" spans="1:5">
       <c r="A65" s="3" t="s">
@@ -1687,15 +1575,11 @@
       <c r="B65" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C65" s="3">
-        <v>4</v>
-      </c>
+      <c r="C65" s="3"/>
       <c r="D65" s="3">
         <v>11</v>
       </c>
-      <c r="E65" s="3">
-        <v>36</v>
-      </c>
+      <c r="E65" s="3"/>
     </row>
     <row r="66" spans="1:5">
       <c r="A66" s="3" t="s">
@@ -1704,15 +1588,11 @@
       <c r="B66" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C66" s="3">
-        <v>1</v>
-      </c>
+      <c r="C66" s="3"/>
       <c r="D66" s="3">
         <v>5</v>
       </c>
-      <c r="E66" s="3">
-        <v>20</v>
-      </c>
+      <c r="E66" s="3"/>
     </row>
     <row r="67" spans="1:5">
       <c r="A67" s="3" t="s">
@@ -1721,15 +1601,11 @@
       <c r="B67" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C67" s="3">
-        <v>1</v>
-      </c>
+      <c r="C67" s="3"/>
       <c r="D67" s="3">
         <v>5</v>
       </c>
-      <c r="E67" s="3">
-        <v>20</v>
-      </c>
+      <c r="E67" s="3"/>
     </row>
     <row r="68" spans="1:5">
       <c r="A68" s="3" t="s">
@@ -1738,15 +1614,11 @@
       <c r="B68" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C68" s="3">
-        <v>2</v>
-      </c>
+      <c r="C68" s="3"/>
       <c r="D68" s="3">
         <v>9</v>
       </c>
-      <c r="E68" s="3">
-        <v>22</v>
-      </c>
+      <c r="E68" s="3"/>
     </row>
     <row r="69" spans="1:5">
       <c r="A69" s="3" t="s">
@@ -1755,15 +1627,11 @@
       <c r="B69" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C69" s="3">
-        <v>2</v>
-      </c>
+      <c r="C69" s="3"/>
       <c r="D69" s="3">
         <v>13</v>
       </c>
-      <c r="E69" s="3">
-        <v>15</v>
-      </c>
+      <c r="E69" s="3"/>
     </row>
     <row r="70" spans="1:5">
       <c r="A70" s="3" t="s">
@@ -1772,15 +1640,11 @@
       <c r="B70" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C70" s="3">
-        <v>3</v>
-      </c>
+      <c r="C70" s="3"/>
       <c r="D70" s="3">
         <v>20</v>
       </c>
-      <c r="E70" s="3">
-        <v>15</v>
-      </c>
+      <c r="E70" s="3"/>
     </row>
     <row r="71" spans="1:5">
       <c r="A71" s="3" t="s">
@@ -1789,15 +1653,11 @@
       <c r="B71" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C71" s="3">
-        <v>1</v>
-      </c>
+      <c r="C71" s="3"/>
       <c r="D71" s="3">
         <v>25</v>
       </c>
-      <c r="E71" s="3">
-        <v>4</v>
-      </c>
+      <c r="E71" s="3"/>
     </row>
     <row r="72" spans="1:5">
       <c r="A72" s="3" t="s">
@@ -1806,15 +1666,11 @@
       <c r="B72" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C72" s="3">
-        <v>2</v>
-      </c>
+      <c r="C72" s="3"/>
       <c r="D72" s="3">
         <v>10</v>
       </c>
-      <c r="E72" s="3">
-        <v>20</v>
-      </c>
+      <c r="E72" s="3"/>
     </row>
     <row r="73" spans="1:5">
       <c r="A73" s="3" t="s">
@@ -1823,15 +1679,11 @@
       <c r="B73" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C73" s="3">
-        <v>1</v>
-      </c>
+      <c r="C73" s="3"/>
       <c r="D73" s="3">
         <v>8</v>
       </c>
-      <c r="E73" s="3">
-        <v>13</v>
-      </c>
+      <c r="E73" s="3"/>
     </row>
     <row r="74" spans="1:5">
       <c r="A74" s="3" t="s">
@@ -1994,15 +1846,11 @@
       <c r="B88" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C88" s="3">
-        <v>1</v>
-      </c>
+      <c r="C88" s="3"/>
       <c r="D88" s="3">
         <v>1</v>
       </c>
-      <c r="E88" s="3">
-        <v>100</v>
-      </c>
+      <c r="E88" s="3"/>
     </row>
     <row r="89" spans="1:5">
       <c r="A89" s="3" t="s">
@@ -2024,15 +1872,11 @@
       <c r="B90" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C90" s="3">
-        <v>1</v>
-      </c>
+      <c r="C90" s="3"/>
       <c r="D90" s="3">
         <v>3</v>
       </c>
-      <c r="E90" s="3">
-        <v>33</v>
-      </c>
+      <c r="E90" s="3"/>
     </row>
     <row r="91" spans="1:5">
       <c r="A91" s="3" t="s">
@@ -2054,15 +1898,11 @@
       <c r="B92" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C92" s="3">
-        <v>1</v>
-      </c>
+      <c r="C92" s="3"/>
       <c r="D92" s="3">
         <v>1</v>
       </c>
-      <c r="E92" s="3">
-        <v>100</v>
-      </c>
+      <c r="E92" s="3"/>
     </row>
     <row r="93" spans="1:5">
       <c r="A93" s="3" t="s">
@@ -2084,15 +1924,11 @@
       <c r="B94" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C94" s="3">
-        <v>3</v>
-      </c>
+      <c r="C94" s="3"/>
       <c r="D94" s="3">
         <v>4</v>
       </c>
-      <c r="E94" s="3">
-        <v>75</v>
-      </c>
+      <c r="E94" s="3"/>
     </row>
     <row r="95" spans="1:5">
       <c r="A95" s="3" t="s">
@@ -2101,15 +1937,11 @@
       <c r="B95" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C95" s="3">
-        <v>3</v>
-      </c>
+      <c r="C95" s="3"/>
       <c r="D95" s="3">
         <v>9</v>
       </c>
-      <c r="E95" s="3">
-        <v>33</v>
-      </c>
+      <c r="E95" s="3"/>
     </row>
     <row r="96" spans="1:5">
       <c r="A96" s="3" t="s">
@@ -2118,9 +1950,7 @@
       <c r="B96" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C96" s="3">
-        <v>1</v>
-      </c>
+      <c r="C96" s="3"/>
       <c r="D96" s="3"/>
       <c r="E96" s="3"/>
     </row>
@@ -2287,9 +2117,7 @@
       <c r="B111" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C111" s="3">
-        <v>1</v>
-      </c>
+      <c r="C111" s="3"/>
       <c r="D111" s="3"/>
       <c r="E111" s="3"/>
     </row>
@@ -2300,15 +2128,11 @@
       <c r="B112" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C112" s="3">
-        <v>1</v>
-      </c>
+      <c r="C112" s="3"/>
       <c r="D112" s="3">
         <v>2</v>
       </c>
-      <c r="E112" s="3">
-        <v>50</v>
-      </c>
+      <c r="E112" s="3"/>
     </row>
     <row r="113" spans="1:5">
       <c r="A113" s="3" t="s">
@@ -2330,15 +2154,11 @@
       <c r="B114" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C114" s="3">
-        <v>1</v>
-      </c>
+      <c r="C114" s="3"/>
       <c r="D114" s="3">
         <v>4</v>
       </c>
-      <c r="E114" s="3">
-        <v>25</v>
-      </c>
+      <c r="E114" s="3"/>
     </row>
     <row r="115" spans="1:5">
       <c r="A115" s="3" t="s">
@@ -2347,15 +2167,11 @@
       <c r="B115" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C115" s="3">
-        <v>1</v>
-      </c>
+      <c r="C115" s="3"/>
       <c r="D115" s="3">
         <v>6</v>
       </c>
-      <c r="E115" s="3">
-        <v>17</v>
-      </c>
+      <c r="E115" s="3"/>
     </row>
     <row r="116" spans="1:5">
       <c r="A116" s="3" t="s">
@@ -2364,15 +2180,11 @@
       <c r="B116" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C116" s="3">
-        <v>2</v>
-      </c>
+      <c r="C116" s="3"/>
       <c r="D116" s="3">
         <v>7</v>
       </c>
-      <c r="E116" s="3">
-        <v>29</v>
-      </c>
+      <c r="E116" s="3"/>
     </row>
     <row r="117" spans="1:5">
       <c r="A117" s="3" t="s">
@@ -2381,15 +2193,11 @@
       <c r="B117" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C117" s="3">
-        <v>1</v>
-      </c>
+      <c r="C117" s="3"/>
       <c r="D117" s="3">
         <v>20</v>
       </c>
-      <c r="E117" s="3">
-        <v>5</v>
-      </c>
+      <c r="E117" s="3"/>
     </row>
     <row r="118" spans="1:5">
       <c r="A118" s="3" t="s">
@@ -2398,15 +2206,11 @@
       <c r="B118" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C118" s="3">
-        <v>3</v>
-      </c>
+      <c r="C118" s="3"/>
       <c r="D118" s="3">
         <v>16</v>
       </c>
-      <c r="E118" s="3">
-        <v>19</v>
-      </c>
+      <c r="E118" s="3"/>
     </row>
     <row r="119" spans="1:5">
       <c r="A119" s="3" t="s">
@@ -2441,15 +2245,11 @@
       <c r="B121" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C121" s="3">
-        <v>1</v>
-      </c>
+      <c r="C121" s="3"/>
       <c r="D121" s="3">
         <v>7</v>
       </c>
-      <c r="E121" s="3">
-        <v>14</v>
-      </c>
+      <c r="E121" s="3"/>
     </row>
     <row r="122" spans="1:5">
       <c r="A122" s="3" t="s">
@@ -2612,15 +2412,11 @@
       <c r="B136" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C136" s="3">
-        <v>1</v>
-      </c>
+      <c r="C136" s="3"/>
       <c r="D136" s="3">
         <v>1</v>
       </c>
-      <c r="E136" s="3">
-        <v>100</v>
-      </c>
+      <c r="E136" s="3"/>
     </row>
     <row r="137" spans="1:5">
       <c r="A137" s="3" t="s">
@@ -2668,15 +2464,11 @@
       <c r="B140" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C140" s="3">
-        <v>1</v>
-      </c>
+      <c r="C140" s="3"/>
       <c r="D140" s="3">
         <v>4</v>
       </c>
-      <c r="E140" s="3">
-        <v>25</v>
-      </c>
+      <c r="E140" s="3"/>
     </row>
     <row r="141" spans="1:5">
       <c r="A141" s="3" t="s">
@@ -2698,15 +2490,11 @@
       <c r="B142" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C142" s="3">
-        <v>1</v>
-      </c>
+      <c r="C142" s="3"/>
       <c r="D142" s="3">
         <v>5</v>
       </c>
-      <c r="E142" s="3">
-        <v>20</v>
-      </c>
+      <c r="E142" s="3"/>
     </row>
     <row r="143" spans="1:5">
       <c r="A143" s="3" t="s">
@@ -2715,15 +2503,11 @@
       <c r="B143" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C143" s="3">
-        <v>1</v>
-      </c>
+      <c r="C143" s="3"/>
       <c r="D143" s="3">
         <v>6</v>
       </c>
-      <c r="E143" s="3">
-        <v>17</v>
-      </c>
+      <c r="E143" s="3"/>
     </row>
     <row r="144" spans="1:5">
       <c r="A144" s="3" t="s">
@@ -2745,15 +2529,11 @@
       <c r="B145" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C145" s="3">
-        <v>1</v>
-      </c>
+      <c r="C145" s="3"/>
       <c r="D145" s="3">
         <v>2</v>
       </c>
-      <c r="E145" s="3">
-        <v>50</v>
-      </c>
+      <c r="E145" s="3"/>
     </row>
     <row r="146" spans="1:5">
       <c r="A146" s="3" t="s">
@@ -2905,9 +2685,7 @@
       <c r="B159" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C159" s="3">
-        <v>1</v>
-      </c>
+      <c r="C159" s="3"/>
       <c r="D159" s="3"/>
       <c r="E159" s="3"/>
     </row>
@@ -2918,15 +2696,11 @@
       <c r="B160" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C160" s="3">
-        <v>2</v>
-      </c>
+      <c r="C160" s="3"/>
       <c r="D160" s="3">
         <v>4</v>
       </c>
-      <c r="E160" s="3">
-        <v>50</v>
-      </c>
+      <c r="E160" s="3"/>
     </row>
     <row r="161" spans="1:5">
       <c r="A161" s="3" t="s">
@@ -2935,15 +2709,11 @@
       <c r="B161" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C161" s="3">
-        <v>2</v>
-      </c>
+      <c r="C161" s="3"/>
       <c r="D161" s="3">
         <v>6</v>
       </c>
-      <c r="E161" s="3">
-        <v>33</v>
-      </c>
+      <c r="E161" s="3"/>
     </row>
     <row r="162" spans="1:5">
       <c r="A162" s="3" t="s">
@@ -2978,15 +2748,11 @@
       <c r="B164" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C164" s="3">
-        <v>1</v>
-      </c>
+      <c r="C164" s="3"/>
       <c r="D164" s="3">
         <v>4</v>
       </c>
-      <c r="E164" s="3">
-        <v>25</v>
-      </c>
+      <c r="E164" s="3"/>
     </row>
     <row r="165" spans="1:5">
       <c r="A165" s="3" t="s">
@@ -2995,15 +2761,11 @@
       <c r="B165" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C165" s="3">
-        <v>4</v>
-      </c>
+      <c r="C165" s="3"/>
       <c r="D165" s="3">
         <v>6</v>
       </c>
-      <c r="E165" s="3">
-        <v>67</v>
-      </c>
+      <c r="E165" s="3"/>
     </row>
     <row r="166" spans="1:5">
       <c r="A166" s="3" t="s">
@@ -3012,15 +2774,11 @@
       <c r="B166" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C166" s="3">
-        <v>3</v>
-      </c>
+      <c r="C166" s="3"/>
       <c r="D166" s="3">
         <v>6</v>
       </c>
-      <c r="E166" s="3">
-        <v>50</v>
-      </c>
+      <c r="E166" s="3"/>
     </row>
     <row r="167" spans="1:5">
       <c r="A167" s="3" t="s">
@@ -3029,15 +2787,11 @@
       <c r="B167" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C167" s="3">
-        <v>1</v>
-      </c>
+      <c r="C167" s="3"/>
       <c r="D167" s="3">
         <v>6</v>
       </c>
-      <c r="E167" s="3">
-        <v>17</v>
-      </c>
+      <c r="E167" s="3"/>
     </row>
     <row r="168" spans="1:5">
       <c r="A168" s="3" t="s">
@@ -3046,9 +2800,7 @@
       <c r="B168" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C168" s="3">
-        <v>1</v>
-      </c>
+      <c r="C168" s="3"/>
       <c r="D168" s="3"/>
       <c r="E168" s="3"/>
     </row>
@@ -3213,9 +2965,7 @@
       <c r="B183" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C183" s="3">
-        <v>1</v>
-      </c>
+      <c r="C183" s="3"/>
       <c r="D183" s="3"/>
       <c r="E183" s="3"/>
     </row>
@@ -3252,15 +3002,11 @@
       <c r="B186" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C186" s="3">
-        <v>3</v>
-      </c>
+      <c r="C186" s="3"/>
       <c r="D186" s="3">
         <v>16</v>
       </c>
-      <c r="E186" s="3">
-        <v>19</v>
-      </c>
+      <c r="E186" s="3"/>
     </row>
     <row r="187" spans="1:5">
       <c r="A187" s="3" t="s">
@@ -3282,15 +3028,11 @@
       <c r="B188" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C188" s="3">
-        <v>1</v>
-      </c>
+      <c r="C188" s="3"/>
       <c r="D188" s="3">
         <v>6</v>
       </c>
-      <c r="E188" s="3">
-        <v>17</v>
-      </c>
+      <c r="E188" s="3"/>
     </row>
     <row r="189" spans="1:5">
       <c r="A189" s="3" t="s">
@@ -3312,15 +3054,11 @@
       <c r="B190" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C190" s="3">
-        <v>1</v>
-      </c>
+      <c r="C190" s="3"/>
       <c r="D190" s="3">
         <v>9</v>
       </c>
-      <c r="E190" s="3">
-        <v>11</v>
-      </c>
+      <c r="E190" s="3"/>
     </row>
     <row r="191" spans="1:5">
       <c r="A191" s="3" t="s">
@@ -3329,15 +3067,11 @@
       <c r="B191" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C191" s="3">
-        <v>1</v>
-      </c>
+      <c r="C191" s="3"/>
       <c r="D191" s="3">
         <v>9</v>
       </c>
-      <c r="E191" s="3">
-        <v>11</v>
-      </c>
+      <c r="E191" s="3"/>
     </row>
     <row r="192" spans="1:5">
       <c r="A192" s="3" t="s">
@@ -3346,15 +3080,11 @@
       <c r="B192" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C192" s="3">
-        <v>2</v>
-      </c>
+      <c r="C192" s="3"/>
       <c r="D192" s="3">
         <v>14</v>
       </c>
-      <c r="E192" s="3">
-        <v>14</v>
-      </c>
+      <c r="E192" s="3"/>
     </row>
     <row r="193" spans="1:5">
       <c r="A193" s="3" t="s">
@@ -3363,15 +3093,11 @@
       <c r="B193" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C193" s="3">
-        <v>2</v>
-      </c>
+      <c r="C193" s="3"/>
       <c r="D193" s="3">
         <v>4</v>
       </c>
-      <c r="E193" s="3">
-        <v>50</v>
-      </c>
+      <c r="E193" s="3"/>
     </row>
     <row r="194" spans="1:5">
       <c r="A194" s="3" t="s">
@@ -3523,9 +3249,7 @@
       <c r="B207" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C207" s="3">
-        <v>1</v>
-      </c>
+      <c r="C207" s="3"/>
       <c r="D207" s="3"/>
       <c r="E207" s="3"/>
     </row>
@@ -3536,15 +3260,11 @@
       <c r="B208" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C208" s="3">
-        <v>2</v>
-      </c>
+      <c r="C208" s="3"/>
       <c r="D208" s="3">
         <v>1</v>
       </c>
-      <c r="E208" s="3">
-        <v>200</v>
-      </c>
+      <c r="E208" s="3"/>
     </row>
     <row r="209" spans="1:5">
       <c r="A209" s="3" t="s">
@@ -3579,15 +3299,11 @@
       <c r="B211" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C211" s="3">
-        <v>1</v>
-      </c>
+      <c r="C211" s="3"/>
       <c r="D211" s="3">
         <v>2</v>
       </c>
-      <c r="E211" s="3">
-        <v>50</v>
-      </c>
+      <c r="E211" s="3"/>
     </row>
     <row r="212" spans="1:5">
       <c r="A212" s="3" t="s">
@@ -3596,15 +3312,11 @@
       <c r="B212" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C212" s="3">
-        <v>2</v>
-      </c>
+      <c r="C212" s="3"/>
       <c r="D212" s="3">
         <v>6</v>
       </c>
-      <c r="E212" s="3">
-        <v>33</v>
-      </c>
+      <c r="E212" s="3"/>
     </row>
     <row r="213" spans="1:5">
       <c r="A213" s="3" t="s">
@@ -3613,15 +3325,11 @@
       <c r="B213" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C213" s="3">
-        <v>3</v>
-      </c>
+      <c r="C213" s="3"/>
       <c r="D213" s="3">
         <v>9</v>
       </c>
-      <c r="E213" s="3">
-        <v>33</v>
-      </c>
+      <c r="E213" s="3"/>
     </row>
     <row r="214" spans="1:5">
       <c r="A214" s="3" t="s">
@@ -3643,15 +3351,11 @@
       <c r="B215" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C215" s="3">
-        <v>1</v>
-      </c>
+      <c r="C215" s="3"/>
       <c r="D215" s="3">
         <v>2</v>
       </c>
-      <c r="E215" s="3">
-        <v>50</v>
-      </c>
+      <c r="E215" s="3"/>
     </row>
     <row r="216" spans="1:5">
       <c r="A216" s="3" t="s">
@@ -3673,9 +3377,7 @@
       <c r="B217" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C217" s="3">
-        <v>1</v>
-      </c>
+      <c r="C217" s="3"/>
       <c r="D217" s="3"/>
       <c r="E217" s="3"/>
     </row>
@@ -3840,15 +3542,11 @@
       <c r="B232" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C232" s="3">
-        <v>1</v>
-      </c>
+      <c r="C232" s="3"/>
       <c r="D232" s="3">
         <v>2</v>
       </c>
-      <c r="E232" s="3">
-        <v>50</v>
-      </c>
+      <c r="E232" s="3"/>
     </row>
     <row r="233" spans="1:5">
       <c r="A233" s="3" t="s">
@@ -3870,15 +3568,11 @@
       <c r="B234" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C234" s="3">
-        <v>1</v>
-      </c>
+      <c r="C234" s="3"/>
       <c r="D234" s="3">
         <v>4</v>
       </c>
-      <c r="E234" s="3">
-        <v>25</v>
-      </c>
+      <c r="E234" s="3"/>
     </row>
     <row r="235" spans="1:5">
       <c r="A235" s="3" t="s">
@@ -3900,15 +3594,11 @@
       <c r="B236" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C236" s="3">
-        <v>1</v>
-      </c>
+      <c r="C236" s="3"/>
       <c r="D236" s="3">
         <v>6</v>
       </c>
-      <c r="E236" s="3">
-        <v>17</v>
-      </c>
+      <c r="E236" s="3"/>
     </row>
     <row r="237" spans="1:5">
       <c r="A237" s="3" t="s">
@@ -3917,15 +3607,11 @@
       <c r="B237" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C237" s="3">
-        <v>2</v>
-      </c>
+      <c r="C237" s="3"/>
       <c r="D237" s="3">
         <v>11</v>
       </c>
-      <c r="E237" s="3">
-        <v>18</v>
-      </c>
+      <c r="E237" s="3"/>
     </row>
     <row r="238" spans="1:5">
       <c r="A238" s="3" t="s">
@@ -3960,15 +3646,11 @@
       <c r="B240" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C240" s="3">
-        <v>2</v>
-      </c>
+      <c r="C240" s="3"/>
       <c r="D240" s="3">
         <v>10</v>
       </c>
-      <c r="E240" s="3">
-        <v>20</v>
-      </c>
+      <c r="E240" s="3"/>
     </row>
     <row r="241" spans="1:5">
       <c r="A241" s="3" t="s">
@@ -3977,15 +3659,11 @@
       <c r="B241" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C241" s="3">
-        <v>3</v>
-      </c>
+      <c r="C241" s="3"/>
       <c r="D241" s="3">
         <v>7</v>
       </c>
-      <c r="E241" s="3">
-        <v>43</v>
-      </c>
+      <c r="E241" s="3"/>
     </row>
     <row r="242" spans="1:5">
       <c r="A242" s="3" t="s">
@@ -4164,15 +3842,11 @@
       <c r="B256" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C256" s="3">
-        <v>1</v>
-      </c>
+      <c r="C256" s="3"/>
       <c r="D256" s="3">
         <v>5</v>
       </c>
-      <c r="E256" s="3">
-        <v>20</v>
-      </c>
+      <c r="E256" s="3"/>
     </row>
     <row r="257" spans="1:5">
       <c r="A257" s="3" t="s">
@@ -4181,15 +3855,11 @@
       <c r="B257" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C257" s="3">
-        <v>2</v>
-      </c>
+      <c r="C257" s="3"/>
       <c r="D257" s="3">
         <v>9</v>
       </c>
-      <c r="E257" s="3">
-        <v>22</v>
-      </c>
+      <c r="E257" s="3"/>
     </row>
     <row r="258" spans="1:5">
       <c r="A258" s="3" t="s">
@@ -4222,9 +3892,7 @@
       <c r="B260" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C260" s="3">
-        <v>2</v>
-      </c>
+      <c r="C260" s="3"/>
       <c r="D260" s="3"/>
       <c r="E260" s="3"/>
     </row>
@@ -4235,9 +3903,7 @@
       <c r="B261" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C261" s="3">
-        <v>2</v>
-      </c>
+      <c r="C261" s="3"/>
       <c r="D261" s="3"/>
       <c r="E261" s="3"/>
     </row>
@@ -4248,9 +3914,7 @@
       <c r="B262" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C262" s="3">
-        <v>2</v>
-      </c>
+      <c r="C262" s="3"/>
       <c r="D262" s="3"/>
       <c r="E262" s="3"/>
     </row>
@@ -4261,9 +3925,7 @@
       <c r="B263" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C263" s="3">
-        <v>1</v>
-      </c>
+      <c r="C263" s="3"/>
       <c r="D263" s="3"/>
       <c r="E263" s="3"/>
     </row>
@@ -4285,9 +3947,7 @@
       <c r="B265" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C265" s="3">
-        <v>1</v>
-      </c>
+      <c r="C265" s="3"/>
       <c r="D265" s="3"/>
       <c r="E265" s="3"/>
     </row>
@@ -4452,15 +4112,11 @@
       <c r="B280" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C280" s="3">
-        <v>1</v>
-      </c>
+      <c r="C280" s="3"/>
       <c r="D280" s="3">
         <v>1</v>
       </c>
-      <c r="E280" s="3">
-        <v>100</v>
-      </c>
+      <c r="E280" s="3"/>
     </row>
     <row r="281" spans="1:5">
       <c r="A281" s="3" t="s">
@@ -4482,15 +4138,11 @@
       <c r="B282" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C282" s="3">
-        <v>1</v>
-      </c>
+      <c r="C282" s="3"/>
       <c r="D282" s="3">
         <v>11</v>
       </c>
-      <c r="E282" s="3">
-        <v>9</v>
-      </c>
+      <c r="E282" s="3"/>
     </row>
     <row r="283" spans="1:5">
       <c r="A283" s="3" t="s">
@@ -4499,15 +4151,11 @@
       <c r="B283" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C283" s="3">
-        <v>2</v>
-      </c>
+      <c r="C283" s="3"/>
       <c r="D283" s="3">
         <v>7</v>
       </c>
-      <c r="E283" s="3">
-        <v>29</v>
-      </c>
+      <c r="E283" s="3"/>
     </row>
     <row r="284" spans="1:5">
       <c r="A284" s="3" t="s">
@@ -4529,15 +4177,11 @@
       <c r="B285" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C285" s="3">
-        <v>3</v>
-      </c>
+      <c r="C285" s="3"/>
       <c r="D285" s="3">
         <v>4</v>
       </c>
-      <c r="E285" s="3">
-        <v>75</v>
-      </c>
+      <c r="E285" s="3"/>
     </row>
     <row r="286" spans="1:5">
       <c r="A286" s="3" t="s">
@@ -4546,15 +4190,11 @@
       <c r="B286" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C286" s="3">
-        <v>1</v>
-      </c>
+      <c r="C286" s="3"/>
       <c r="D286" s="3">
         <v>18</v>
       </c>
-      <c r="E286" s="3">
-        <v>6</v>
-      </c>
+      <c r="E286" s="3"/>
     </row>
     <row r="287" spans="1:5">
       <c r="A287" s="3" t="s">
@@ -4563,15 +4203,11 @@
       <c r="B287" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C287" s="3">
-        <v>1</v>
-      </c>
+      <c r="C287" s="3"/>
       <c r="D287" s="3">
         <v>6</v>
       </c>
-      <c r="E287" s="3">
-        <v>17</v>
-      </c>
+      <c r="E287" s="3"/>
     </row>
     <row r="288" spans="1:5">
       <c r="A288" s="3" t="s">
@@ -4580,15 +4216,11 @@
       <c r="B288" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C288" s="3">
-        <v>3</v>
-      </c>
+      <c r="C288" s="3"/>
       <c r="D288" s="3">
         <v>10</v>
       </c>
-      <c r="E288" s="3">
-        <v>30</v>
-      </c>
+      <c r="E288" s="3"/>
     </row>
     <row r="289" spans="1:5">
       <c r="A289" s="3" t="s">
@@ -4597,15 +4229,11 @@
       <c r="B289" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C289" s="3">
-        <v>1</v>
-      </c>
+      <c r="C289" s="3"/>
       <c r="D289" s="3">
         <v>3</v>
       </c>
-      <c r="E289" s="3">
-        <v>33</v>
-      </c>
+      <c r="E289" s="3"/>
     </row>
     <row r="290" spans="1:5">
       <c r="A290" s="3" t="s">
@@ -4757,9 +4385,7 @@
       <c r="B303" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C303" s="3">
-        <v>1</v>
-      </c>
+      <c r="C303" s="3"/>
       <c r="D303" s="3"/>
       <c r="E303" s="3"/>
     </row>
@@ -4770,9 +4396,7 @@
       <c r="B304" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C304" s="3">
-        <v>1</v>
-      </c>
+      <c r="C304" s="3"/>
       <c r="D304" s="3"/>
       <c r="E304" s="3"/>
     </row>
@@ -4877,9 +4501,7 @@
       <c r="B313" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C313" s="3">
-        <v>1</v>
-      </c>
+      <c r="C313" s="3"/>
       <c r="D313" s="3"/>
       <c r="E313" s="3"/>
     </row>
@@ -5052,15 +4674,11 @@
       <c r="B328" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C328" s="3">
-        <v>1</v>
-      </c>
+      <c r="C328" s="3"/>
       <c r="D328" s="3">
         <v>3</v>
       </c>
-      <c r="E328" s="3">
-        <v>33</v>
-      </c>
+      <c r="E328" s="3"/>
     </row>
     <row r="329" spans="1:5">
       <c r="A329" s="3" t="s">
@@ -5108,15 +4726,11 @@
       <c r="B332" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C332" s="3">
-        <v>2</v>
-      </c>
+      <c r="C332" s="3"/>
       <c r="D332" s="3">
         <v>6</v>
       </c>
-      <c r="E332" s="3">
-        <v>33</v>
-      </c>
+      <c r="E332" s="3"/>
     </row>
     <row r="333" spans="1:5">
       <c r="A333" s="3" t="s">
@@ -5125,15 +4739,11 @@
       <c r="B333" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C333" s="3">
-        <v>1</v>
-      </c>
+      <c r="C333" s="3"/>
       <c r="D333" s="3">
         <v>5</v>
       </c>
-      <c r="E333" s="3">
-        <v>20</v>
-      </c>
+      <c r="E333" s="3"/>
     </row>
     <row r="334" spans="1:5">
       <c r="A334" s="3" t="s">
@@ -5181,9 +4791,7 @@
       <c r="B337" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C337" s="3">
-        <v>1</v>
-      </c>
+      <c r="C337" s="3"/>
       <c r="D337" s="3"/>
       <c r="E337" s="3"/>
     </row>

</xml_diff>